<commit_message>
Update docs and example spreadsheets
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/family_history_template.xlsx
+++ b/docs/public/help/help_linked_docs/family_history_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/Documents/help_linked_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{951BF75D-FB08-9E49-8C5E-54EEB523E007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC734EA7-3C6D-7A46-9D96-588D5C45DC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="17440" xr2:uid="{265770E1-D1B3-004D-B7B5-9ABB68F7FE7E}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Individual ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Mother ID</t>
   </si>
@@ -36,86 +33,126 @@
     <t>Father ID</t>
   </si>
   <si>
-    <t>MONDO terms</t>
-  </si>
-  <si>
-    <t>Proband</t>
-  </si>
-  <si>
     <t>Clinical Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Family ID </t>
-  </si>
-  <si>
     <t>Ancestry</t>
   </si>
   <si>
-    <t>Life status</t>
-  </si>
-  <si>
     <t>Deceased</t>
   </si>
   <si>
-    <t>Cause of death</t>
-  </si>
-  <si>
-    <t>Age at death</t>
-  </si>
-  <si>
-    <t>Age at death units</t>
-  </si>
-  <si>
     <t>Pregnancy</t>
   </si>
   <si>
-    <t>Gestational age</t>
-  </si>
-  <si>
-    <t>Is termination of pregnancy</t>
-  </si>
-  <si>
-    <t>Spontaneous abortion</t>
-  </si>
-  <si>
-    <t>Still birth</t>
-  </si>
-  <si>
-    <t>No children by choice</t>
-  </si>
-  <si>
     <t>Infertile</t>
   </si>
   <si>
-    <t>Cause of infertility</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Gestational age units</t>
-  </si>
-  <si>
-    <t>HPO terms</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
     <t>Age Units</t>
+  </si>
+  <si>
+    <t>Family ID*</t>
+  </si>
+  <si>
+    <t>Individual ID*</t>
+  </si>
+  <si>
+    <t>Sex*</t>
+  </si>
+  <si>
+    <t>Proband*</t>
+  </si>
+  <si>
+    <t>Primary Diagnosis</t>
+  </si>
+  <si>
+    <t>Diagnosis Age of Onset</t>
+  </si>
+  <si>
+    <t>Diagnosis Age of Onset Units</t>
+  </si>
+  <si>
+    <t>Diagnostic Confidence</t>
+  </si>
+  <si>
+    <t>HPO Terms</t>
+  </si>
+  <si>
+    <t>MONDO Terms</t>
+  </si>
+  <si>
+    <t>Life Status</t>
+  </si>
+  <si>
+    <t>Cause of Death</t>
+  </si>
+  <si>
+    <t>Age at Death</t>
+  </si>
+  <si>
+    <t>Age at Death Units</t>
+  </si>
+  <si>
+    <t>Gestational Age</t>
+  </si>
+  <si>
+    <t>Gestational Age Units</t>
+  </si>
+  <si>
+    <t>Is Termination of Pregnancy</t>
+  </si>
+  <si>
+    <t>Spontaneous Abortion</t>
+  </si>
+  <si>
+    <t>Still Birth</t>
+  </si>
+  <si>
+    <t>No Children by Choice</t>
+  </si>
+  <si>
+    <t>Cause of Infertility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,14 +175,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBC60BD-0E12-D44C-BBC2-53BF1D50CDD5}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -471,105 +513,127 @@
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
     <col min="19" max="20" width="15.42578125" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" customWidth="1"/>
-    <col min="23" max="23" width="9" customWidth="1"/>
-    <col min="25" max="25" width="8.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" customWidth="1"/>
+    <col min="25" max="25" width="25.42578125" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" customWidth="1"/>
+    <col min="30" max="30" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:31" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="AD1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1" tooltip="Click to search for HPO terms" xr:uid="{3EE5D431-9D15-974E-B61E-76BCBC06E2D2}"/>
+    <hyperlink ref="H1" r:id="rId2" tooltip="Click to search for MONDO terms" xr:uid="{F100797F-D90E-B042-8788-9477F867CE99}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update docs, example files
Also, some small tweaks to handle errors found during testing.
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/family_history_template.xlsx
+++ b/docs/public/help/help_linked_docs/family_history_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC734EA7-3C6D-7A46-9D96-588D5C45DC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAB1A94-80FF-1D4C-927E-75FA7B889F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="17440" xr2:uid="{265770E1-D1B3-004D-B7B5-9ABB68F7FE7E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Mother ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Infertile</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>Diagnostic Confidence</t>
   </si>
   <si>
-    <t>HPO Terms</t>
-  </si>
-  <si>
-    <t>MONDO Terms</t>
-  </si>
-  <si>
     <t>Life Status</t>
   </si>
   <si>
@@ -99,15 +90,6 @@
     <t>Age at Death Units</t>
   </si>
   <si>
-    <t>Gestational Age</t>
-  </si>
-  <si>
-    <t>Gestational Age Units</t>
-  </si>
-  <si>
-    <t>Is Termination of Pregnancy</t>
-  </si>
-  <si>
     <t>Spontaneous Abortion</t>
   </si>
   <si>
@@ -118,6 +100,18 @@
   </si>
   <si>
     <t>Cause of Infertility</t>
+  </si>
+  <si>
+    <t>Gestational Age (Weeks)</t>
+  </si>
+  <si>
+    <t>HPO Terms (Phenotypes)</t>
+  </si>
+  <si>
+    <t>MONDO Terms (Disorders)</t>
+  </si>
+  <si>
+    <t>Termination of Pregnancy</t>
   </si>
 </sst>
 </file>
@@ -500,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBC60BD-0E12-D44C-BBC2-53BF1D50CDD5}">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -513,8 +507,8 @@
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="25.42578125" customWidth="1"/>
@@ -527,25 +521,24 @@
     <col min="19" max="20" width="15.42578125" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
-    <col min="24" max="24" width="18.85546875" customWidth="1"/>
-    <col min="25" max="25" width="25.42578125" customWidth="1"/>
-    <col min="26" max="26" width="20.5703125" customWidth="1"/>
-    <col min="30" max="30" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="21.85546875" customWidth="1"/>
+    <col min="24" max="24" width="25.42578125" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -554,28 +547,28 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>2</v>
@@ -584,55 +577,49 @@
         <v>3</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" tooltip="Click to search for HPO terms" xr:uid="{3EE5D431-9D15-974E-B61E-76BCBC06E2D2}"/>
-    <hyperlink ref="H1" r:id="rId2" tooltip="Click to search for MONDO terms" xr:uid="{F100797F-D90E-B042-8788-9477F867CE99}"/>
+    <hyperlink ref="G1" r:id="rId1" tooltip="Click to search for HPO terms" display="HPO Terms" xr:uid="{3EE5D431-9D15-974E-B61E-76BCBC06E2D2}"/>
+    <hyperlink ref="H1" r:id="rId2" tooltip="Click to search for MONDO terms" display="MONDO Terms" xr:uid="{F100797F-D90E-B042-8788-9477F867CE99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix column name and add drop down option
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/family_history_template.xlsx
+++ b/docs/public/help/help_linked_docs/family_history_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAB1A94-80FF-1D4C-927E-75FA7B889F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4724C098-5C7F-9048-8DD8-270A174E2C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="17440" xr2:uid="{265770E1-D1B3-004D-B7B5-9ABB68F7FE7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +33,6 @@
     <t>Father ID</t>
   </si>
   <si>
-    <t>Clinical Notes</t>
-  </si>
-  <si>
     <t>Ancestry</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Termination of Pregnancy</t>
+  </si>
+  <si>
+    <t>Clinic Notes</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBC60BD-0E12-D44C-BBC2-53BF1D50CDD5}">
   <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -529,16 +529,16 @@
   <sheetData>
     <row r="1" spans="1:29" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -547,73 +547,73 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add birth year to family history docs + templates
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/family_history_template.xlsx
+++ b/docs/public/help/help_linked_docs/family_history_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal-2/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4724C098-5C7F-9048-8DD8-270A174E2C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2130F-88D9-F84C-8CEC-EF9E2A6810C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="17440" xr2:uid="{265770E1-D1B3-004D-B7B5-9ABB68F7FE7E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Mother ID</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Clinic Notes</t>
+  </si>
+  <si>
+    <t>Birth Year</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBC60BD-0E12-D44C-BBC2-53BF1D50CDD5}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -514,20 +517,20 @@
     <col min="11" max="11" width="25.42578125" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="19" max="20" width="15.42578125" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="21.85546875" customWidth="1"/>
-    <col min="24" max="24" width="25.42578125" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" customWidth="1"/>
+    <col min="14" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="20" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" customWidth="1"/>
+    <col min="25" max="25" width="25.42578125" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" customWidth="1"/>
+    <col min="30" max="30" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -571,48 +574,51 @@
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>